<commit_message>
3inchx8mm file added in A645
</commit_message>
<xml_diff>
--- a/System_development/magnet_design/A320_Tesla_magnet/A320_BillofMaterials.xlsx
+++ b/System_development/magnet_design/A320_Tesla_magnet/A320_BillofMaterials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adowney2\Documents\GitHub\Compact-NMR\System_development\magnet_design\A320_Tesla_magnet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usman\OneDrive - Georgia Southern University\Desktop\USC-1stSemester\NMR\Compact-NMR\System_development\magnet_design\A320_Tesla_magnet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F9B72B-5725-44B4-9259-842A09F82912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102FBE6B-F69C-4483-8F8B-D774F4AE8D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BillofMaterials" sheetId="1" r:id="rId1"/>
@@ -74,9 +74,6 @@
     <t>Vendor 4</t>
   </si>
   <si>
-    <t>3 x 1 Inch Neodymium Rare Earth Disc Magnet N42 DZ0X0</t>
-  </si>
-  <si>
     <t>Iron Face Plate</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>NN52 square Disc Magnet</t>
+  </si>
+  <si>
+    <t>3 x 3 x 1/4 Inch Neodymium Rare Earth Block Magnet N52</t>
   </si>
 </sst>
 </file>
@@ -986,25 +986,25 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="39" customWidth="1"/>
-    <col min="7" max="7" width="47.1328125" customWidth="1"/>
+    <col min="7" max="7" width="47.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1054,12 +1054,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
         <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1072,15 +1072,15 @@
         <v>190.64</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1092,46 +1092,46 @@
         <v>17.43</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D18" s="3"/>
     </row>
   </sheetData>

</xml_diff>